<commit_message>
chore: update treasury bulk upload and output templates
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\OneDrive - ICF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B12FD3D-4E08-420F-BF53-0B8A52C35624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C8E7C-81B6-48E4-B49F-7324161499B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Template Name: SLFRF Broadband Location Template</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>The FCC-provided ID that will align with the entity that files or will file Broadband Data Collection data</t>
-  </si>
-  <si>
-    <t>Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
   </si>
   <si>
     <t>Enter the latitude data for the location to which service is installed.
@@ -216,6 +213,31 @@
   </si>
   <si>
     <t>Version: 2023.5.25</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>[DO NOT ENTER FOR EXISTING ENTRIES]
+Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DO NOT ENTER FOR NEW ENTRIES] This is a Treasury Portal auto-generated unique ID only for used when updating existing locations in bulk upload. The IDs can be found in the “My Broadband Locations” table as well as through the “Download as CSV” feature. </t>
+  </si>
+  <si>
+    <t>Void_Location__c</t>
+  </si>
+  <si>
+    <t>Void Location</t>
+  </si>
+  <si>
+    <t>Not required. If the location is no longer relevant, set this column to 'Void' to remove it from the displayed locations. Locations will default to 'Display'.
+Options: 
+'Void'
+'Display'</t>
   </si>
 </sst>
 </file>
@@ -271,13 +293,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -299,14 +324,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +365,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -450,7 +471,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -600,33 +621,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F803400-39A4-425E-BE38-4133E8AD7233}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="32.42578125" style="2"/>
+    <col min="2" max="2" width="35.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="32.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:17" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,54 +659,60 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>48</v>
+      <c r="Q4" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
@@ -693,16 +724,16 @@
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>29</v>
@@ -711,16 +742,22 @@
         <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -728,90 +765,102 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="Q6" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="339.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="339.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "chore: update treasury bulk upload and output templates"
This reverts commit dbc321b23279e337bbf97441d59268fcbe9c7b0e.
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\OneDrive - ICF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C8E7C-81B6-48E4-B49F-7324161499B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B12FD3D-4E08-420F-BF53-0B8A52C35624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Template Name: SLFRF Broadband Location Template</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>The FCC-provided ID that will align with the entity that files or will file Broadband Data Collection data</t>
+  </si>
+  <si>
+    <t>Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
   </si>
   <si>
     <t>Enter the latitude data for the location to which service is installed.
@@ -213,31 +216,6 @@
   </si>
   <si>
     <t>Version: 2023.5.25</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>[DO NOT ENTER FOR EXISTING ENTRIES]
-Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[DO NOT ENTER FOR NEW ENTRIES] This is a Treasury Portal auto-generated unique ID only for used when updating existing locations in bulk upload. The IDs can be found in the “My Broadband Locations” table as well as through the “Download as CSV” feature. </t>
-  </si>
-  <si>
-    <t>Void_Location__c</t>
-  </si>
-  <si>
-    <t>Void Location</t>
-  </si>
-  <si>
-    <t>Not required. If the location is no longer relevant, set this column to 'Void' to remove it from the displayed locations. Locations will default to 'Display'.
-Options: 
-'Void'
-'Display'</t>
   </si>
 </sst>
 </file>
@@ -293,16 +271,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -324,10 +299,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -365,7 +344,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -471,7 +450,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -613,7 +592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,37 +600,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F803400-39A4-425E-BE38-4133E8AD7233}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="32.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="32.44140625" style="2"/>
+    <col min="2" max="16384" width="32.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3"/>
+    <row r="3" spans="1:15" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,60 +634,54 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
@@ -724,16 +693,16 @@
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>29</v>
@@ -742,22 +711,16 @@
         <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -765,102 +728,90 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="7" spans="1:17" ht="339.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="339.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="P7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update workbook and validation
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/slfrfBroadbandLocationBulkUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\42853\OneDrive - ICF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B12FD3D-4E08-420F-BF53-0B8A52C35624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C8E7C-81B6-48E4-B49F-7324161499B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{4037144D-154C-4ECA-A138-CB4373BF1F03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Template Name: SLFRF Broadband Location Template</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>The FCC-provided ID that will align with the entity that files or will file Broadband Data Collection data</t>
-  </si>
-  <si>
-    <t>Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
   </si>
   <si>
     <t>Enter the latitude data for the location to which service is installed.
@@ -216,6 +213,31 @@
   </si>
   <si>
     <t>Version: 2023.5.25</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>[DO NOT ENTER FOR EXISTING ENTRIES]
+Enter the site specific fabric identification number (Fabric ID) from the FCC broadband funded locations map that corresponds with the location in the field provided. This is the Broadband Serviceable Fabric Location (Max length - 20 characters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[DO NOT ENTER FOR NEW ENTRIES] This is a Treasury Portal auto-generated unique ID only for used when updating existing locations in bulk upload. The IDs can be found in the “My Broadband Locations” table as well as through the “Download as CSV” feature. </t>
+  </si>
+  <si>
+    <t>Void_Location__c</t>
+  </si>
+  <si>
+    <t>Void Location</t>
+  </si>
+  <si>
+    <t>Not required. If the location is no longer relevant, set this column to 'Void' to remove it from the displayed locations. Locations will default to 'Display'.
+Options: 
+'Void'
+'Display'</t>
   </si>
 </sst>
 </file>
@@ -271,13 +293,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -299,14 +324,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,7 +365,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -450,7 +471,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,7 +613,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -600,33 +621,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F803400-39A4-425E-BE38-4133E8AD7233}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="32.42578125" style="2"/>
+    <col min="2" max="2" width="35.77734375" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="32.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="3"/>
+    <row r="3" spans="1:17" ht="151.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,54 +659,60 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>48</v>
+      <c r="Q4" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
@@ -693,16 +724,16 @@
         <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="J5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>29</v>
@@ -711,16 +742,22 @@
         <v>29</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -728,90 +765,102 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="Q6" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" ht="339.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="339.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>